<commit_message>
Fix fixture and row handler
</commit_message>
<xml_diff>
--- a/fixture/src/main/java/domainapp/fixture/scenarios/demo/DemoFixture.xlsx
+++ b/fixture/src/main/java/domainapp/fixture/scenarios/demo/DemoFixture.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jvanderwal\src\github\incodehq\contactapp\fixture\src\main\java\domainapp\fixture\scenarios\demo\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="26835" windowHeight="13110"/>
+    <workbookView xWindow="480" yWindow="132" windowWidth="26832" windowHeight="13116"/>
   </bookViews>
   <sheets>
     <sheet name="ContactRowHandler" sheetId="5" r:id="rId1"/>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="81">
   <si>
     <t>name</t>
   </si>
@@ -100,9 +105,6 @@
     <t>bill.smith@acmecompany.com</t>
   </si>
   <si>
-    <t>ACME HQ</t>
-  </si>
-  <si>
     <t>Bob Mills</t>
   </si>
   <si>
@@ -175,9 +177,6 @@
     <t>d.goodnew@abcdef.nl</t>
   </si>
   <si>
-    <t>ACME - 107 rue Saint Joan, 87654 Paris</t>
-  </si>
-  <si>
     <t>Clarisse Bentz</t>
   </si>
   <si>
@@ -196,9 +195,6 @@
     <t>clarisse.bentz@acmecompany.fr</t>
   </si>
   <si>
-    <t>Somewhere - Or Other - RN 22, 43214 Amiens</t>
-  </si>
-  <si>
     <t>Security-R-Us</t>
   </si>
   <si>
@@ -254,6 +250,18 @@
   </si>
   <si>
     <t>+33 6 90 90 90 90</t>
+  </si>
+  <si>
+    <t>ACME</t>
+  </si>
+  <si>
+    <t>Global</t>
+  </si>
+  <si>
+    <t>Paris Office</t>
+  </si>
+  <si>
+    <t>Amiens Property</t>
   </si>
 </sst>
 </file>
@@ -418,6 +426,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -465,7 +476,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -500,7 +511,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -712,21 +723,21 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="49.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="36.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -758,13 +769,16 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>28</v>
+        <v>78</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="C2" t="s">
+        <v>77</v>
+      </c>
       <c r="D2" s="2" t="s">
         <v>23</v>
       </c>
@@ -781,138 +795,148 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
       <c r="B3" s="1"/>
+      <c r="C3" t="s">
+        <v>77</v>
+      </c>
       <c r="D3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="F3" s="9" t="s">
         <v>30</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>31</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
       <c r="B4" s="1"/>
+      <c r="C4" t="s">
+        <v>77</v>
+      </c>
       <c r="D4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="F4" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="G4" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="H4" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="H4" s="10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
       <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C6" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C6" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" s="4" t="s">
+      <c r="E6" s="11" t="s">
         <v>42</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>43</v>
       </c>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
       <c r="H6" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>22</v>
       </c>
       <c r="D7" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="F7" s="11" t="s">
         <v>46</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>47</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D8" s="4" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D8" s="4" t="s">
+      <c r="E8" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="F8" s="11" t="s">
         <v>50</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>51</v>
       </c>
       <c r="G8" s="4"/>
       <c r="H8" s="10" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C9" s="6"/>
+        <v>79</v>
+      </c>
+      <c r="C9" t="s">
+        <v>77</v>
+      </c>
       <c r="D9" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="E9" s="13" t="s">
-        <v>56</v>
-      </c>
       <c r="F9" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C10" s="7"/>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>77</v>
+      </c>
       <c r="D10" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>13</v>
@@ -922,80 +946,82 @@
       </c>
       <c r="G10" s="7"/>
       <c r="H10" s="15" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C11" s="6"/>
+        <v>80</v>
+      </c>
+      <c r="C11" t="s">
+        <v>77</v>
+      </c>
       <c r="D11" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="13" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="G11" s="6"/>
       <c r="H11" s="17" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="I11" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C12" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F12" s="18" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G12" s="7"/>
       <c r="H12" s="15" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="I12" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C13" s="7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F13" s="18" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G13" s="7"/>
       <c r="H13" s="15" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="I13" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C14" s="7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>18</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
@@ -1004,26 +1030,26 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C15" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
       <c r="H15" s="16" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="I15" s="7" t="s">
         <v>19</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>